<commit_message>
poort A1 vervangen door A2
</commit_message>
<xml_diff>
--- a/instellen-parrameters-ntc.xlsx
+++ b/instellen-parrameters-ntc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriaanbakker/Thermostaatcontroller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9F27709-85CC-A94A-9B42-DEBA1B0953AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FE3A30-482D-2E4E-9409-5C3EFC873080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{14559BB1-9E98-3247-BC52-C91E48C2E679}"/>
+    <workbookView xWindow="880" yWindow="1540" windowWidth="33600" windowHeight="18940" xr2:uid="{14559BB1-9E98-3247-BC52-C91E48C2E679}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,55 +505,55 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>366</v>
+        <v>567</v>
       </c>
       <c r="B2">
         <f>(1023-A2)/A2 *100</f>
-        <v>179.50819672131149</v>
+        <v>80.423280423280417</v>
       </c>
       <c r="C2">
         <f>LN(B2)</f>
-        <v>5.190220871071336</v>
+        <v>4.3873036917747257</v>
       </c>
       <c r="D2">
-        <v>22.4</v>
+        <v>17.8</v>
       </c>
       <c r="E2">
         <f>D2+273.15</f>
-        <v>295.54999999999995</v>
+        <v>290.95</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>230</v>
+        <v>421</v>
       </c>
       <c r="B3">
         <f>(1023-A3)/A3 *100</f>
-        <v>344.78260869565219</v>
+        <v>142.99287410926368</v>
       </c>
       <c r="C3">
         <f>LN(B3)</f>
-        <v>5.8429140986997439</v>
+        <v>4.9627947976145315</v>
       </c>
       <c r="D3">
-        <v>10.8</v>
+        <v>7.1</v>
       </c>
       <c r="E3">
         <f>D3+273.15</f>
-        <v>283.95</v>
+        <v>280.25</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D5">
         <f>E2</f>
-        <v>295.54999999999995</v>
+        <v>290.95</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2">
         <f>C2</f>
-        <v>5.190220871071336</v>
+        <v>4.3873036917747257</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>5</v>
@@ -568,14 +568,14 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D6">
         <f>E3</f>
-        <v>283.95</v>
+        <v>280.25</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="2">
         <f>C3</f>
-        <v>5.8429140986997439</v>
+        <v>4.9627947976145315</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
@@ -602,14 +602,14 @@
       </c>
       <c r="G8" s="2">
         <f>D5*F5</f>
-        <v>1533.9697784451332</v>
+        <v>1276.4860091218563</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I8">
         <f>D5</f>
-        <v>295.54999999999995</v>
+        <v>290.95</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>14</v>
@@ -625,14 +625,14 @@
       </c>
       <c r="G9" s="2">
         <f>F6*D6</f>
-        <v>1659.0954583257922</v>
+        <v>1390.8232420314725</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I9">
         <f>D6</f>
-        <v>283.95</v>
+        <v>280.25</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>14</v>
@@ -647,14 +647,14 @@
       </c>
       <c r="G11" s="2">
         <f>G8-G9</f>
-        <v>-125.12567988065894</v>
+        <v>-114.3372329096162</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I11">
         <f>(I8-I9)</f>
-        <v>11.599999999999966</v>
+        <v>10.699999999999989</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>14</v>
@@ -670,7 +670,7 @@
       </c>
       <c r="F13">
         <f>G11/I11</f>
-        <v>-10.786696541436147</v>
+        <v>-10.685722701833301</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
       </c>
       <c r="F14" s="5">
         <f>EXP(F13)</f>
-        <v>2.0672700563788907E-5</v>
+        <v>2.2869127482606205E-5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
       </c>
       <c r="F15">
         <f>G8-I8*F13</f>
-        <v>4721.9779412665857</v>
+        <v>4385.4970292202552</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -733,11 +733,11 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" ref="D21" si="2">$F$15/(C21-$F$13)</f>
-        <v>295.31366068682615</v>
+        <v>276.01306460456283</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" ref="E21" si="3">D21-273.15</f>
-        <v>22.163660686826177</v>
+        <v>2.8630646045628509</v>
       </c>
       <c r="I21">
         <v>199</v>
@@ -757,11 +757,11 @@
       </c>
       <c r="D22" s="2">
         <f t="shared" ref="D22" si="6">$F$15/(C22-$F$13)</f>
-        <v>287.17567052513397</v>
+        <v>268.3599459409424</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" ref="E22" si="7">D22-273.15</f>
-        <v>14.025670525133989</v>
+        <v>-4.7900540590575815</v>
       </c>
       <c r="I22">
         <v>189</v>
@@ -781,11 +781,11 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" ref="D23" si="10">$F$15/(C23-$F$13)</f>
-        <v>289.77736621749602</v>
+        <v>270.8063379312116</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" ref="E23" si="11">D23-273.15</f>
-        <v>16.627366217496046</v>
+        <v>-2.343662068788376</v>
       </c>
       <c r="I23">
         <v>189</v>

</xml_diff>